<commit_message>
agregando archivos de configuracion
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,28 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\essa-file08\6230-E-TE\BOT'S\Consolidacion de Recaudo - jhon\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{858BBEF2-C873-4D0E-9389-E5743195007D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
     <sheet name="Constants" sheetId="2" r:id="rId2"/>
     <sheet name="Assets" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +130,36 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>UrlSAC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://essa-ws12.essa.com.co:9095/GEN/Vistas/Login/Login_Gen.aspx </t>
+  </si>
+  <si>
+    <t>UsuarioSAC</t>
+  </si>
+  <si>
+    <t>LARIAGIL</t>
+  </si>
+  <si>
+    <t>UrlRecConsigConsultas</t>
+  </si>
+  <si>
+    <t>https://essa-ws12.essa.com.co:9095/SAC/Vistas/App/REC_LOTECO.aspx</t>
+  </si>
+  <si>
+    <t>RutaResultado</t>
+  </si>
+  <si>
+    <t>RutaDescargas</t>
+  </si>
+  <si>
+    <t>C:\Users\jpumarej\Downloads</t>
+  </si>
+  <si>
+    <t>D:\Leidy\Consolidación recaudos</t>
   </si>
 </sst>
 </file>
@@ -173,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -183,6 +221,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -201,7 +240,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -499,16 +538,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -557,7 +596,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="29">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -573,11 +612,46 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
@@ -1574,12 +1648,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1616,7 +1690,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2682,16 +2756,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.1796875" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>